<commit_message>
Added effort commitment snapshot
</commit_message>
<xml_diff>
--- a/docs/budget/effort_committment.xlsx
+++ b/docs/budget/effort_committment.xlsx
@@ -1134,7 +1134,7 @@
       <c r="K17" s="10"/>
       <c r="L17" s="11">
         <f>SUM(E35:L37)</f>
-        <v>71.225</v>
+        <v>147.5375</v>
       </c>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
@@ -1170,7 +1170,7 @@
       <c r="G18" s="12"/>
       <c r="H18" s="13">
         <f>SUM(E35:H37)</f>
-        <v>25.4375</v>
+        <v>55.9625</v>
       </c>
       <c r="I18" s="12" t="s">
         <v>20</v>
@@ -1179,7 +1179,7 @@
       <c r="K18" s="12"/>
       <c r="L18" s="13">
         <f>SUM(I35:L37)</f>
-        <v>45.7875</v>
+        <v>91.575</v>
       </c>
       <c r="M18" s="14" t="s">
         <v>30</v>
@@ -1194,7 +1194,7 @@
       <c r="U18" s="14"/>
       <c r="V18" s="15">
         <f>SUM(M35:V37)</f>
-        <v>126.8375</v>
+        <v>258.675</v>
       </c>
       <c r="W18" s="16" t="s">
         <v>31</v>
@@ -1203,7 +1203,7 @@
       <c r="Y18" s="16"/>
       <c r="Z18" s="17">
         <f>SUM(W35:Z37)</f>
-        <v>171.05</v>
+        <v>337.1</v>
       </c>
       <c r="AA18" s="1"/>
       <c r="AB18" s="1"/>
@@ -1901,22 +1901,22 @@
         <v>24</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="K27" s="3" t="s">
         <v>24</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="M27" s="3" t="s">
         <v>24</v>
@@ -1927,56 +1927,56 @@
       <c r="O27" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="P27" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q27" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="R27" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="S27" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="T27" s="3" t="s">
-        <v>24</v>
+      <c r="P27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="T27" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="U27" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="V27" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="W27" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="X27" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y27" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z27" s="3" t="s">
-        <v>24</v>
+        <v>17</v>
+      </c>
+      <c r="V27" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="W27" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="X27" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y27" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z27" s="23" t="s">
+        <v>21</v>
       </c>
       <c r="AA27" s="1"/>
       <c r="AB27" s="1"/>
       <c r="AC27" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>50.875</v>
       </c>
       <c r="AD27" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>30.2625</v>
       </c>
       <c r="AE27" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>45.2625</v>
       </c>
       <c r="AF27" s="4">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>126.4</v>
       </c>
       <c r="AG27" s="1"/>
     </row>
@@ -1996,22 +1996,22 @@
         <v>24</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="K28" s="3" t="s">
         <v>24</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="M28" s="3" t="s">
         <v>24</v>
@@ -2022,56 +2022,56 @@
       <c r="O28" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="P28" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q28" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="R28" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="S28" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="T28" s="3" t="s">
-        <v>24</v>
+      <c r="P28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="T28" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="U28" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="V28" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="W28" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="X28" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y28" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z28" s="3" t="s">
-        <v>24</v>
+        <v>13</v>
+      </c>
+      <c r="V28" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="W28" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="X28" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y28" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z28" s="23" t="s">
+        <v>21</v>
       </c>
       <c r="AA28" s="1"/>
       <c r="AB28" s="1"/>
       <c r="AC28" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>55.9625</v>
       </c>
       <c r="AD28" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>20.175</v>
       </c>
       <c r="AE28" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>45.2625</v>
       </c>
       <c r="AF28" s="4">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>121.4</v>
       </c>
       <c r="AG28" s="1"/>
     </row>
@@ -2091,22 +2091,22 @@
         <v>24</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="K29" s="3" t="s">
         <v>24</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="M29" s="3" t="s">
         <v>24</v>
@@ -2117,56 +2117,56 @@
       <c r="O29" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="P29" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q29" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="R29" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="S29" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="T29" s="3" t="s">
-        <v>24</v>
+      <c r="P29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="T29" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="U29" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="V29" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="W29" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="X29" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y29" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z29" s="3" t="s">
-        <v>24</v>
+        <v>17</v>
+      </c>
+      <c r="V29" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="W29" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="X29" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y29" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z29" s="23" t="s">
+        <v>21</v>
       </c>
       <c r="AA29" s="1"/>
       <c r="AB29" s="1"/>
       <c r="AC29" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>50.875</v>
       </c>
       <c r="AD29" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>30.2625</v>
       </c>
       <c r="AE29" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>45.2625</v>
       </c>
       <c r="AF29" s="4">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>126.4</v>
       </c>
       <c r="AG29" s="1"/>
     </row>
@@ -2597,19 +2597,19 @@
       </c>
       <c r="G35" s="4">
         <f t="shared" si="7"/>
-        <v>10.175</v>
+        <v>25.4375</v>
       </c>
       <c r="H35" s="4">
         <f t="shared" si="7"/>
-        <v>15.2625</v>
+        <v>30.525</v>
       </c>
       <c r="I35" s="4">
         <f t="shared" si="7"/>
-        <v>15.2625</v>
+        <v>30.525</v>
       </c>
       <c r="J35" s="4">
         <f t="shared" si="7"/>
-        <v>15.2625</v>
+        <v>30.525</v>
       </c>
       <c r="K35" s="4">
         <f t="shared" si="7"/>
@@ -2617,7 +2617,7 @@
       </c>
       <c r="L35" s="4">
         <f t="shared" si="7"/>
-        <v>15.2625</v>
+        <v>30.525</v>
       </c>
       <c r="M35" s="4">
         <f t="shared" si="7"/>
@@ -2633,27 +2633,27 @@
       </c>
       <c r="P35" s="4">
         <f t="shared" si="7"/>
-        <v>15.2625</v>
+        <v>30.525</v>
       </c>
       <c r="Q35" s="4">
         <f t="shared" si="7"/>
-        <v>15.2625</v>
+        <v>30.525</v>
       </c>
       <c r="R35" s="4">
         <f t="shared" si="7"/>
-        <v>15.2625</v>
+        <v>30.525</v>
       </c>
       <c r="S35" s="4">
         <f t="shared" si="7"/>
-        <v>15.2625</v>
+        <v>30.525</v>
       </c>
       <c r="T35" s="4">
         <f t="shared" si="7"/>
-        <v>15.2625</v>
+        <v>30.525</v>
       </c>
       <c r="U35" s="4">
         <f t="shared" si="7"/>
-        <v>10.175</v>
+        <v>15.2625</v>
       </c>
       <c r="V35" s="4">
         <f t="shared" si="7"/>
@@ -2757,15 +2757,15 @@
       </c>
       <c r="U36" s="4">
         <f t="shared" si="9"/>
-        <v>10.0875</v>
+        <v>30.2625</v>
       </c>
       <c r="V36" s="4">
         <f t="shared" si="9"/>
-        <v>30.2625</v>
+        <v>60.525</v>
       </c>
       <c r="W36" s="4">
         <f t="shared" si="9"/>
-        <v>10.0875</v>
+        <v>40.35</v>
       </c>
       <c r="X36" s="4">
         <f t="shared" si="9"/>
@@ -2785,19 +2785,19 @@
       </c>
       <c r="AC36" s="18">
         <f t="shared" ref="AC36:AF36" si="10">SUM(AC24:AC34)</f>
-        <v>157.7125</v>
+        <v>315.425</v>
       </c>
       <c r="AD36" s="18">
         <f t="shared" si="10"/>
-        <v>60.525</v>
+        <v>141.225</v>
       </c>
       <c r="AE36" s="18">
         <f t="shared" si="10"/>
-        <v>150.875</v>
+        <v>286.6625</v>
       </c>
       <c r="AF36" s="18">
         <f t="shared" si="10"/>
-        <v>369.1125</v>
+        <v>743.3125</v>
       </c>
       <c r="AG36" s="18" t="s">
         <v>5</v>
@@ -2889,15 +2889,15 @@
       </c>
       <c r="X37" s="4">
         <f t="shared" si="11"/>
-        <v>30.175</v>
+        <v>75.4375</v>
       </c>
       <c r="Y37" s="4">
         <f t="shared" si="11"/>
-        <v>45.2625</v>
+        <v>90.525</v>
       </c>
       <c r="Z37" s="4">
         <f t="shared" si="11"/>
-        <v>45.2625</v>
+        <v>90.525</v>
       </c>
       <c r="AA37" s="4"/>
       <c r="AB37" s="4"/>
@@ -3066,19 +3066,19 @@
       </c>
       <c r="G42" s="4">
         <f t="shared" si="12"/>
-        <v>10.175</v>
+        <v>25.4375</v>
       </c>
       <c r="H42" s="4">
         <f t="shared" si="12"/>
-        <v>15.2625</v>
+        <v>30.525</v>
       </c>
       <c r="I42" s="4">
         <f t="shared" si="12"/>
-        <v>15.2625</v>
+        <v>30.525</v>
       </c>
       <c r="J42" s="4">
         <f t="shared" si="12"/>
-        <v>15.2625</v>
+        <v>30.525</v>
       </c>
       <c r="K42" s="4">
         <f t="shared" si="12"/>
@@ -3086,7 +3086,7 @@
       </c>
       <c r="L42" s="4">
         <f t="shared" si="12"/>
-        <v>15.2625</v>
+        <v>30.525</v>
       </c>
       <c r="M42" s="4">
         <f t="shared" si="12"/>
@@ -3102,47 +3102,47 @@
       </c>
       <c r="P42" s="4">
         <f t="shared" si="12"/>
-        <v>15.2625</v>
+        <v>30.525</v>
       </c>
       <c r="Q42" s="4">
         <f t="shared" si="12"/>
-        <v>15.2625</v>
+        <v>30.525</v>
       </c>
       <c r="R42" s="4">
         <f t="shared" si="12"/>
-        <v>15.2625</v>
+        <v>30.525</v>
       </c>
       <c r="S42" s="4">
         <f t="shared" si="12"/>
-        <v>15.2625</v>
+        <v>30.525</v>
       </c>
       <c r="T42" s="4">
         <f t="shared" si="12"/>
-        <v>15.2625</v>
+        <v>30.525</v>
       </c>
       <c r="U42" s="4">
         <f t="shared" si="12"/>
-        <v>20.2625</v>
+        <v>45.525</v>
       </c>
       <c r="V42" s="4">
         <f t="shared" si="12"/>
-        <v>30.2625</v>
+        <v>60.525</v>
       </c>
       <c r="W42" s="4">
         <f t="shared" si="12"/>
-        <v>40.2625</v>
+        <v>70.525</v>
       </c>
       <c r="X42" s="4">
         <f t="shared" si="12"/>
-        <v>40.2625</v>
+        <v>85.525</v>
       </c>
       <c r="Y42" s="4">
         <f t="shared" si="12"/>
-        <v>45.2625</v>
+        <v>90.525</v>
       </c>
       <c r="Z42" s="4">
         <f t="shared" si="12"/>
-        <v>45.2625</v>
+        <v>90.525</v>
       </c>
       <c r="AA42" s="4"/>
       <c r="AB42" s="18" t="s">
@@ -3152,7 +3152,7 @@
       <c r="AD42" s="18"/>
       <c r="AE42" s="18">
         <f>SUM(E42:Z42)</f>
-        <v>369.1125</v>
+        <v>743.3125</v>
       </c>
       <c r="AF42" s="18"/>
       <c r="AG42" s="18" t="s">
@@ -3176,17 +3176,17 @@
       <c r="G43" s="4"/>
       <c r="H43" s="4">
         <f>SUM(G42:H42)</f>
-        <v>25.4375</v>
+        <v>55.9625</v>
       </c>
       <c r="I43" s="4"/>
       <c r="J43" s="4">
         <f>SUM(I42:J42)</f>
-        <v>30.525</v>
+        <v>61.05</v>
       </c>
       <c r="K43" s="4"/>
       <c r="L43" s="4">
         <f>SUM(K42:L42)</f>
-        <v>15.2625</v>
+        <v>30.525</v>
       </c>
       <c r="M43" s="4"/>
       <c r="N43" s="4">
@@ -3196,32 +3196,32 @@
       <c r="O43" s="4"/>
       <c r="P43" s="4">
         <f>SUM(O42:P42)</f>
-        <v>15.2625</v>
+        <v>30.525</v>
       </c>
       <c r="Q43" s="4"/>
       <c r="R43" s="4">
         <f>SUM(Q42:R42)</f>
-        <v>30.525</v>
+        <v>61.05</v>
       </c>
       <c r="S43" s="4"/>
       <c r="T43" s="4">
         <f>SUM(S42:T42)</f>
-        <v>30.525</v>
+        <v>61.05</v>
       </c>
       <c r="U43" s="4"/>
       <c r="V43" s="4">
         <f>SUM(U42:V42)</f>
-        <v>50.525</v>
+        <v>106.05</v>
       </c>
       <c r="W43" s="4"/>
       <c r="X43" s="4">
         <f>SUM(W42:X42)</f>
-        <v>80.525</v>
+        <v>156.05</v>
       </c>
       <c r="Y43" s="4"/>
       <c r="Z43" s="4">
         <f>SUM(Y42:Z42)</f>
-        <v>90.525</v>
+        <v>181.05</v>
       </c>
       <c r="AA43" s="4"/>
       <c r="AB43" s="18" t="s">
@@ -3231,7 +3231,7 @@
       <c r="AD43" s="18"/>
       <c r="AE43" s="18">
         <f>SUM(D43:Z43)</f>
-        <v>369.1125</v>
+        <v>743.3125</v>
       </c>
       <c r="AF43" s="4"/>
       <c r="AG43" s="18" t="s">
@@ -3350,7 +3350,7 @@
       </c>
       <c r="C47" s="30">
         <f>AE43</f>
-        <v>369.1125</v>
+        <v>743.3125</v>
       </c>
       <c r="D47" s="31" t="s">
         <v>54</v>
@@ -36969,19 +36969,19 @@
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P24:R29 S24:U27 V24:Z29">
+  <conditionalFormatting sqref="P24:Z29">
     <cfRule type="cellIs" dxfId="0" priority="39" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P24:R29 S24:U27 V24:Z29">
+  <conditionalFormatting sqref="P24:Z29">
     <cfRule type="cellIs" dxfId="1" priority="40" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P24:R29 S24:U27 V24:Z29">
+  <conditionalFormatting sqref="P24:Z29">
     <cfRule type="cellIs" dxfId="2" priority="41" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>

</xml_diff>